<commit_message>
added demo images, hunger scale
</commit_message>
<xml_diff>
--- a/demoImageList.xlsx
+++ b/demoImageList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Experiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9853BBA4-BA8D-4849-9EC7-BFDD9976CF10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D23D52FE-6EEB-4418-AF55-3D4BA0AA91AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4340" yWindow="2840" windowWidth="12280" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8210" yWindow="830" windowWidth="12280" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -70,24 +70,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
-    <t>images/Caucasian/baconEggCheese.jpg</t>
-  </si>
-  <si>
-    <t>baconEggCheese.jpg</t>
-  </si>
-  <si>
-    <t>images/Caucasian/bagel.jpg</t>
-  </si>
-  <si>
-    <t>bagel.jpg</t>
-  </si>
-  <si>
-    <t>images/Caucasian/balogneSandwhich.jpg</t>
-  </si>
-  <si>
-    <t>balogneSandwhich.jpg</t>
-  </si>
-  <si>
     <t>ImageName</t>
   </si>
   <si>
@@ -98,6 +80,24 @@
   </si>
   <si>
     <t>ImageFile</t>
+  </si>
+  <si>
+    <t>images/Demo/paisa platter.jpg</t>
+  </si>
+  <si>
+    <t>paisa platter.jpg</t>
+  </si>
+  <si>
+    <t>empanada.jpeg</t>
+  </si>
+  <si>
+    <t>images/Demo/empanada.jpeg</t>
+  </si>
+  <si>
+    <t>tamales.jpg</t>
+  </si>
+  <si>
+    <t>images/Demo/tamales.jpg</t>
   </si>
 </sst>
 </file>
@@ -535,7 +535,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7265625" defaultRowHeight="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -546,46 +546,46 @@
   <sheetData>
     <row r="1" spans="1:3" s="3" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
         <v>2</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
@@ -611,21 +611,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B9F5CAB0486A994CA2C3B13E059EF2AE" ma:contentTypeVersion="0" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="8645ec4a60d0c8c7009d2d6675847a91">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="636d7205651659ec4fcda0bcbde9384b">
     <xsd:element name="properties">
@@ -739,30 +724,22 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3725960-8A89-4E70-9C40-340E0EDB6403}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3744155D-8FAB-4E67-B5E0-C7FDBFB3715D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EFF1C174-6AC6-4774-A736-3226A12360E4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -776,4 +753,27 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3744155D-8FAB-4E67-B5E0-C7FDBFB3715D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3725960-8A89-4E70-9C40-340E0EDB6403}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>